<commit_message>
Added park locations and revised map
</commit_message>
<xml_diff>
--- a/Ward49.xlsx
+++ b/Ward49.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="83">
   <si>
     <t>name</t>
   </si>
@@ -46,7 +46,10 @@
     <t>url</t>
   </si>
   <si>
-    <t>location_type</t>
+    <t>loc_type_pri</t>
+  </si>
+  <si>
+    <t>loc_type_sec</t>
   </si>
   <si>
     <t>Rogers Park</t>
@@ -76,6 +79,72 @@
     <t>NEW FIELD</t>
   </si>
   <si>
+    <t>HARTIGAN (DAVID) BEACH</t>
+  </si>
+  <si>
+    <t>HOWARD (URE) BEACH</t>
+  </si>
+  <si>
+    <t>GRIFFIN (MARION MAHONY) BEACH</t>
+  </si>
+  <si>
+    <t>LANGDON (MARY MARGARET)</t>
+  </si>
+  <si>
+    <t>LAZARUS (EMMA)</t>
+  </si>
+  <si>
+    <t>LEONE (SAM) BEACH</t>
+  </si>
+  <si>
+    <t>LOYOLA</t>
+  </si>
+  <si>
+    <t>COLUMBIA BEACH</t>
+  </si>
+  <si>
+    <t>MATANKY (EUGENE)</t>
+  </si>
+  <si>
+    <t>FARGO (JAMES) BEACH</t>
+  </si>
+  <si>
+    <t>GOLDBERG (LOUIS)</t>
+  </si>
+  <si>
+    <t>PASCHEN (CHRISTIAN)</t>
+  </si>
+  <si>
+    <t>WHITE (WILLYE B.)</t>
+  </si>
+  <si>
+    <t>POTTAWATTOMIE</t>
+  </si>
+  <si>
+    <t>JUNEWAY TERR. BEACH</t>
+  </si>
+  <si>
+    <t>PRINZ (TOBEY) BEACH</t>
+  </si>
+  <si>
+    <t>NORTH SHORE BEACH</t>
+  </si>
+  <si>
+    <t>ROGERS (PHILLIP) BEACH</t>
+  </si>
+  <si>
+    <t>TOUHY (PATRICK)</t>
+  </si>
+  <si>
+    <t>WASHINGTON (HAROLD) MEM.</t>
+  </si>
+  <si>
+    <t>TRIANGLE</t>
+  </si>
+  <si>
+    <t>DUBKIN (LEONARD)</t>
+  </si>
+  <si>
     <t>6907 N. Clark St.</t>
   </si>
   <si>
@@ -124,10 +193,76 @@
     <t>Library</t>
   </si>
   <si>
+    <t>School</t>
+  </si>
+  <si>
+    <t>Park</t>
+  </si>
+  <si>
     <t>High School</t>
   </si>
   <si>
     <t>Elementary School</t>
+  </si>
+  <si>
+    <t>PLAYGROUND</t>
+  </si>
+  <si>
+    <t>BEACH</t>
+  </si>
+  <si>
+    <t>PLAYGROUND PARK</t>
+  </si>
+  <si>
+    <t>GYMNASIUM</t>
+  </si>
+  <si>
+    <t>BASKETBALL COURT</t>
+  </si>
+  <si>
+    <t>FOOTBALL/SOCCER COMBO FLD</t>
+  </si>
+  <si>
+    <t>BASEBALL JR/SOFTBALL</t>
+  </si>
+  <si>
+    <t>BASEBALL SR</t>
+  </si>
+  <si>
+    <t>TENNIS COURT</t>
+  </si>
+  <si>
+    <t>BOAT LAUNCH NON-MOTORIZED</t>
+  </si>
+  <si>
+    <t>SHUFFLEBOARD</t>
+  </si>
+  <si>
+    <t>BOXING CENTER</t>
+  </si>
+  <si>
+    <t>VOLLEYBALL</t>
+  </si>
+  <si>
+    <t>HANDBALL/RACQUET (IN)</t>
+  </si>
+  <si>
+    <t>DOG FRIENDLY AREA</t>
+  </si>
+  <si>
+    <t>ARTIFICIAL TURF FIELD</t>
+  </si>
+  <si>
+    <t>NATURE/BIRD SANCTUARY</t>
+  </si>
+  <si>
+    <t>FITNESS CENTER</t>
+  </si>
+  <si>
+    <t>SPRAY FEATURE</t>
+  </si>
+  <si>
+    <t>COMMUNITY GARDEN</t>
   </si>
 </sst>
 </file>
@@ -498,13 +633,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,28 +673,31 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="H2">
         <v>42.00670763656976</v>
@@ -568,18 +706,21 @@
         <v>-87.6734076726854</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>58</v>
+      </c>
+      <c r="L2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H3">
         <v>42.00268756</v>
@@ -588,15 +729,18 @@
         <v>-87.66919215</v>
       </c>
       <c r="K3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>59</v>
+      </c>
+      <c r="L3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="H4">
         <v>42.02109056</v>
@@ -605,15 +749,18 @@
         <v>-87.67193897999999</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>59</v>
+      </c>
+      <c r="L4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="H5">
         <v>42.01647588</v>
@@ -622,15 +769,18 @@
         <v>-87.68440568</v>
       </c>
       <c r="K5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>59</v>
+      </c>
+      <c r="L5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="H6">
         <v>42.00966386</v>
@@ -639,15 +789,18 @@
         <v>-87.6699854</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>59</v>
+      </c>
+      <c r="L6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="H7">
         <v>42.01708759</v>
@@ -656,15 +809,18 @@
         <v>-87.67776252</v>
       </c>
       <c r="K7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>59</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="H8">
         <v>42.01303149</v>
@@ -673,15 +829,18 @@
         <v>-87.67481841999999</v>
       </c>
       <c r="K8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+        <v>59</v>
+      </c>
+      <c r="L8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="H9">
         <v>42.00364046</v>
@@ -690,15 +849,18 @@
         <v>-87.66822247</v>
       </c>
       <c r="K9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>59</v>
+      </c>
+      <c r="L9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="H10">
         <v>42.00770257</v>
@@ -707,7 +869,996 @@
         <v>-87.67316833</v>
       </c>
       <c r="K10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11">
+        <v>42.002272</v>
+      </c>
+      <c r="I11">
+        <v>-87.65769376</v>
+      </c>
+      <c r="K11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12">
+        <v>42.01886353</v>
+      </c>
+      <c r="I12">
+        <v>-87.66391455</v>
+      </c>
+      <c r="K12" t="s">
+        <v>60</v>
+      </c>
+      <c r="L12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13">
+        <v>42.01907479</v>
+      </c>
+      <c r="I13">
+        <v>-87.66424859999999</v>
+      </c>
+      <c r="K13" t="s">
+        <v>60</v>
+      </c>
+      <c r="L13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14">
+        <v>42.0158813</v>
+      </c>
+      <c r="I14">
+        <v>-87.66262924999999</v>
+      </c>
+      <c r="K14" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="H15">
+        <v>42.00188401</v>
+      </c>
+      <c r="I15">
+        <v>-87.67487409</v>
+      </c>
+      <c r="K15" t="s">
+        <v>60</v>
+      </c>
+      <c r="L15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16">
+        <v>42.00417767</v>
+      </c>
+      <c r="I16">
+        <v>-87.66319003</v>
+      </c>
+      <c r="K16" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17">
+        <v>42.01313386</v>
+      </c>
+      <c r="I17">
+        <v>-87.66156823999999</v>
+      </c>
+      <c r="K17" t="s">
+        <v>60</v>
+      </c>
+      <c r="L17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18">
+        <v>42.01316429</v>
+      </c>
+      <c r="I18">
+        <v>-87.66253502000001</v>
+      </c>
+      <c r="K18" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19">
+        <v>42.01318998</v>
+      </c>
+      <c r="I19">
+        <v>-87.66316225999999</v>
+      </c>
+      <c r="K19" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20">
+        <v>42.0123889</v>
+      </c>
+      <c r="I20">
+        <v>-87.66170244</v>
+      </c>
+      <c r="K20" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21">
+        <v>42.00976787</v>
+      </c>
+      <c r="I21">
+        <v>-87.65909651</v>
+      </c>
+      <c r="K21" t="s">
+        <v>60</v>
+      </c>
+      <c r="L21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22">
+        <v>42.00726255</v>
+      </c>
+      <c r="I22">
+        <v>-87.6584077</v>
+      </c>
+      <c r="K22" t="s">
+        <v>60</v>
+      </c>
+      <c r="L22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23">
+        <v>42.01089057</v>
+      </c>
+      <c r="I23">
+        <v>-87.66159962</v>
+      </c>
+      <c r="K23" t="s">
+        <v>60</v>
+      </c>
+      <c r="L23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="H24">
+        <v>42.01221106</v>
+      </c>
+      <c r="I24">
+        <v>-87.66248470000001</v>
+      </c>
+      <c r="K24" t="s">
+        <v>60</v>
+      </c>
+      <c r="L24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25">
+        <v>42.01089571</v>
+      </c>
+      <c r="I25">
+        <v>-87.66061040000001</v>
+      </c>
+      <c r="K25" t="s">
+        <v>60</v>
+      </c>
+      <c r="L25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26">
+        <v>42.01122718</v>
+      </c>
+      <c r="I26">
+        <v>-87.66208738</v>
+      </c>
+      <c r="K26" t="s">
+        <v>60</v>
+      </c>
+      <c r="L26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27">
+        <v>42.00644341</v>
+      </c>
+      <c r="I27">
+        <v>-87.65816288000001</v>
+      </c>
+      <c r="K27" t="s">
+        <v>60</v>
+      </c>
+      <c r="L27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28">
+        <v>42.01300795</v>
+      </c>
+      <c r="I28">
+        <v>-87.66221625</v>
+      </c>
+      <c r="K28" t="s">
+        <v>60</v>
+      </c>
+      <c r="L28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29">
+        <v>42.00448795</v>
+      </c>
+      <c r="I29">
+        <v>-87.65723976</v>
+      </c>
+      <c r="K29" t="s">
+        <v>60</v>
+      </c>
+      <c r="L29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="H30">
+        <v>42.00742796</v>
+      </c>
+      <c r="I30">
+        <v>-87.68052475</v>
+      </c>
+      <c r="K30" t="s">
+        <v>60</v>
+      </c>
+      <c r="L30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <v>42.01708142</v>
+      </c>
+      <c r="I31">
+        <v>-87.66303859999999</v>
+      </c>
+      <c r="K31" t="s">
+        <v>60</v>
+      </c>
+      <c r="L31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32">
+        <v>42.01066244</v>
+      </c>
+      <c r="I32">
+        <v>-87.66565974</v>
+      </c>
+      <c r="K32" t="s">
+        <v>60</v>
+      </c>
+      <c r="L32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33">
+        <v>42.01059159</v>
+      </c>
+      <c r="I33">
+        <v>-87.66033019</v>
+      </c>
+      <c r="K33" t="s">
+        <v>60</v>
+      </c>
+      <c r="L33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34">
+        <v>42.01093076</v>
+      </c>
+      <c r="I34">
+        <v>-87.66139119</v>
+      </c>
+      <c r="K34" t="s">
+        <v>60</v>
+      </c>
+      <c r="L34" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="H35">
+        <v>42.00911792</v>
+      </c>
+      <c r="I35">
+        <v>-87.67972193999999</v>
+      </c>
+      <c r="K35" t="s">
+        <v>60</v>
+      </c>
+      <c r="L35" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36">
+        <v>42.01973153</v>
+      </c>
+      <c r="I36">
+        <v>-87.67151174999999</v>
+      </c>
+      <c r="K36" t="s">
+        <v>60</v>
+      </c>
+      <c r="L36" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+      <c r="H37">
+        <v>42.0151835</v>
+      </c>
+      <c r="I37">
+        <v>-87.67813995</v>
+      </c>
+      <c r="K37" t="s">
+        <v>60</v>
+      </c>
+      <c r="L37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38">
+        <v>42.01703857</v>
+      </c>
+      <c r="I38">
+        <v>-87.67673435</v>
+      </c>
+      <c r="K38" t="s">
+        <v>60</v>
+      </c>
+      <c r="L38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+      <c r="H39">
+        <v>42.0152869</v>
+      </c>
+      <c r="I39">
+        <v>-87.67867489</v>
+      </c>
+      <c r="K39" t="s">
+        <v>60</v>
+      </c>
+      <c r="L39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" t="s">
+        <v>27</v>
+      </c>
+      <c r="H40">
+        <v>42.00665408</v>
+      </c>
+      <c r="I40">
+        <v>-87.65640562</v>
+      </c>
+      <c r="K40" t="s">
+        <v>60</v>
+      </c>
+      <c r="L40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41">
+        <v>42.02244483</v>
+      </c>
+      <c r="I41">
+        <v>-87.66522105</v>
+      </c>
+      <c r="K41" t="s">
+        <v>60</v>
+      </c>
+      <c r="L41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="H42">
+        <v>42.00589177</v>
+      </c>
+      <c r="I42">
+        <v>-87.65748605</v>
+      </c>
+      <c r="K42" t="s">
+        <v>60</v>
+      </c>
+      <c r="L42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" t="s">
         <v>37</v>
+      </c>
+      <c r="H43">
+        <v>42.00403506</v>
+      </c>
+      <c r="I43">
+        <v>-87.65734402</v>
+      </c>
+      <c r="K43" t="s">
+        <v>60</v>
+      </c>
+      <c r="L43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44">
+        <v>42.00916848</v>
+      </c>
+      <c r="I44">
+        <v>-87.67992694</v>
+      </c>
+      <c r="K44" t="s">
+        <v>60</v>
+      </c>
+      <c r="L44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45">
+        <v>42.00916859</v>
+      </c>
+      <c r="I45">
+        <v>-87.67950729</v>
+      </c>
+      <c r="K45" t="s">
+        <v>60</v>
+      </c>
+      <c r="L45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" t="s">
+        <v>34</v>
+      </c>
+      <c r="H46">
+        <v>42.01542812</v>
+      </c>
+      <c r="I46">
+        <v>-87.67757895</v>
+      </c>
+      <c r="K46" t="s">
+        <v>60</v>
+      </c>
+      <c r="L46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" t="s">
+        <v>34</v>
+      </c>
+      <c r="H47">
+        <v>42.01610979</v>
+      </c>
+      <c r="I47">
+        <v>-87.67716962</v>
+      </c>
+      <c r="K47" t="s">
+        <v>60</v>
+      </c>
+      <c r="L47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" t="s">
+        <v>34</v>
+      </c>
+      <c r="H48">
+        <v>42.01512649</v>
+      </c>
+      <c r="I48">
+        <v>-87.67810622</v>
+      </c>
+      <c r="K48" t="s">
+        <v>60</v>
+      </c>
+      <c r="L48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" t="s">
+        <v>34</v>
+      </c>
+      <c r="H49">
+        <v>42.01524922</v>
+      </c>
+      <c r="I49">
+        <v>-87.67820733000001</v>
+      </c>
+      <c r="K49" t="s">
+        <v>60</v>
+      </c>
+      <c r="L49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="H50">
+        <v>42.01585245</v>
+      </c>
+      <c r="I50">
+        <v>-87.67648475</v>
+      </c>
+      <c r="K50" t="s">
+        <v>60</v>
+      </c>
+      <c r="L50" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12">
+      <c r="A51" t="s">
+        <v>34</v>
+      </c>
+      <c r="H51">
+        <v>42.01478544</v>
+      </c>
+      <c r="I51">
+        <v>-87.67859150000001</v>
+      </c>
+      <c r="K51" t="s">
+        <v>60</v>
+      </c>
+      <c r="L51" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12">
+      <c r="A52" t="s">
+        <v>34</v>
+      </c>
+      <c r="H52">
+        <v>42.01494665</v>
+      </c>
+      <c r="I52">
+        <v>-87.67857954999999</v>
+      </c>
+      <c r="K52" t="s">
+        <v>60</v>
+      </c>
+      <c r="L52" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="A53" t="s">
+        <v>34</v>
+      </c>
+      <c r="H53">
+        <v>42.01573372</v>
+      </c>
+      <c r="I53">
+        <v>-87.67788145999999</v>
+      </c>
+      <c r="K53" t="s">
+        <v>60</v>
+      </c>
+      <c r="L53" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+      <c r="H54">
+        <v>42.02148479</v>
+      </c>
+      <c r="I54">
+        <v>-87.66471496</v>
+      </c>
+      <c r="K54" t="s">
+        <v>60</v>
+      </c>
+      <c r="L54" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12">
+      <c r="A55" t="s">
+        <v>38</v>
+      </c>
+      <c r="H55">
+        <v>42.02090483</v>
+      </c>
+      <c r="I55">
+        <v>-87.66456614000001</v>
+      </c>
+      <c r="K55" t="s">
+        <v>60</v>
+      </c>
+      <c r="L55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12">
+      <c r="A56" t="s">
+        <v>39</v>
+      </c>
+      <c r="H56">
+        <v>42.01483425</v>
+      </c>
+      <c r="I56">
+        <v>-87.67360098</v>
+      </c>
+      <c r="K56" t="s">
+        <v>60</v>
+      </c>
+      <c r="L56" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" t="s">
+        <v>39</v>
+      </c>
+      <c r="H57">
+        <v>42.01450382</v>
+      </c>
+      <c r="I57">
+        <v>-87.67386432000001</v>
+      </c>
+      <c r="K57" t="s">
+        <v>60</v>
+      </c>
+      <c r="L57" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="A58" t="s">
+        <v>39</v>
+      </c>
+      <c r="H58">
+        <v>42.01564025</v>
+      </c>
+      <c r="I58">
+        <v>-87.67275167</v>
+      </c>
+      <c r="K58" t="s">
+        <v>60</v>
+      </c>
+      <c r="L58" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" t="s">
+        <v>39</v>
+      </c>
+      <c r="H59">
+        <v>42.01408016</v>
+      </c>
+      <c r="I59">
+        <v>-87.67465871</v>
+      </c>
+      <c r="K59" t="s">
+        <v>60</v>
+      </c>
+      <c r="L59" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="A60" t="s">
+        <v>40</v>
+      </c>
+      <c r="H60">
+        <v>42.02149093</v>
+      </c>
+      <c r="I60">
+        <v>-87.67338743000001</v>
+      </c>
+      <c r="K60" t="s">
+        <v>60</v>
+      </c>
+      <c r="L60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="A61" t="s">
+        <v>33</v>
+      </c>
+      <c r="H61">
+        <v>42.01991204</v>
+      </c>
+      <c r="I61">
+        <v>-87.67154392</v>
+      </c>
+      <c r="K61" t="s">
+        <v>60</v>
+      </c>
+      <c r="L61" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12">
+      <c r="A62" t="s">
+        <v>33</v>
+      </c>
+      <c r="H62">
+        <v>42.01966568</v>
+      </c>
+      <c r="I62">
+        <v>-87.67032349999999</v>
+      </c>
+      <c r="K62" t="s">
+        <v>60</v>
+      </c>
+      <c r="L62" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+      <c r="H63">
+        <v>42.02021117</v>
+      </c>
+      <c r="I63">
+        <v>-87.67091352</v>
+      </c>
+      <c r="K63" t="s">
+        <v>60</v>
+      </c>
+      <c r="L63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12">
+      <c r="A64" t="s">
+        <v>33</v>
+      </c>
+      <c r="H64">
+        <v>42.01968231</v>
+      </c>
+      <c r="I64">
+        <v>-87.67136621</v>
+      </c>
+      <c r="K64" t="s">
+        <v>60</v>
+      </c>
+      <c r="L64" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="A65" t="s">
+        <v>41</v>
+      </c>
+      <c r="H65">
+        <v>42.02254257</v>
+      </c>
+      <c r="I65">
+        <v>-87.67446021000001</v>
+      </c>
+      <c r="K65" t="s">
+        <v>60</v>
+      </c>
+      <c r="L65" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="H66">
+        <v>42.0174474</v>
+      </c>
+      <c r="I66">
+        <v>-87.67065533</v>
+      </c>
+      <c r="K66" t="s">
+        <v>60</v>
+      </c>
+      <c r="L66" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" t="s">
+        <v>31</v>
+      </c>
+      <c r="H67">
+        <v>42.01050482</v>
+      </c>
+      <c r="I67">
+        <v>-87.665638</v>
+      </c>
+      <c r="K67" t="s">
+        <v>60</v>
+      </c>
+      <c r="L67" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="A68" t="s">
+        <v>27</v>
+      </c>
+      <c r="H68">
+        <v>42.00763449</v>
+      </c>
+      <c r="I68">
+        <v>-87.65960633</v>
+      </c>
+      <c r="K68" t="s">
+        <v>60</v>
+      </c>
+      <c r="L68" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added fire stations and fixed uppercase fields
</commit_message>
<xml_diff>
--- a/Ward49.xlsx
+++ b/Ward49.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="85">
   <si>
     <t>name</t>
   </si>
@@ -55,121 +55,127 @@
     <t>Rogers Park</t>
   </si>
   <si>
-    <t>SULLIVAN HS</t>
-  </si>
-  <si>
-    <t>GALE</t>
-  </si>
-  <si>
-    <t>ACERO - DE LA CRUZ</t>
-  </si>
-  <si>
-    <t>FIELD</t>
-  </si>
-  <si>
-    <t>JORDAN</t>
-  </si>
-  <si>
-    <t>CHICAGO MATH &amp; SCIENCE HS</t>
-  </si>
-  <si>
-    <t>KILMER</t>
-  </si>
-  <si>
-    <t>NEW FIELD</t>
-  </si>
-  <si>
-    <t>HARTIGAN (DAVID) BEACH</t>
-  </si>
-  <si>
-    <t>HOWARD (URE) BEACH</t>
-  </si>
-  <si>
-    <t>GRIFFIN (MARION MAHONY) BEACH</t>
-  </si>
-  <si>
-    <t>LANGDON (MARY MARGARET)</t>
-  </si>
-  <si>
-    <t>LAZARUS (EMMA)</t>
-  </si>
-  <si>
-    <t>LEONE (SAM) BEACH</t>
-  </si>
-  <si>
-    <t>LOYOLA</t>
-  </si>
-  <si>
-    <t>COLUMBIA BEACH</t>
-  </si>
-  <si>
-    <t>MATANKY (EUGENE)</t>
-  </si>
-  <si>
-    <t>FARGO (JAMES) BEACH</t>
-  </si>
-  <si>
-    <t>GOLDBERG (LOUIS)</t>
-  </si>
-  <si>
-    <t>PASCHEN (CHRISTIAN)</t>
-  </si>
-  <si>
-    <t>WHITE (WILLYE B.)</t>
-  </si>
-  <si>
-    <t>POTTAWATTOMIE</t>
-  </si>
-  <si>
-    <t>JUNEWAY TERR. BEACH</t>
-  </si>
-  <si>
-    <t>PRINZ (TOBEY) BEACH</t>
-  </si>
-  <si>
-    <t>NORTH SHORE BEACH</t>
-  </si>
-  <si>
-    <t>ROGERS (PHILLIP) BEACH</t>
-  </si>
-  <si>
-    <t>TOUHY (PATRICK)</t>
-  </si>
-  <si>
-    <t>WASHINGTON (HAROLD) MEM.</t>
-  </si>
-  <si>
-    <t>TRIANGLE</t>
-  </si>
-  <si>
-    <t>DUBKIN (LEONARD)</t>
+    <t>Sullivan Hs</t>
+  </si>
+  <si>
+    <t>Gale</t>
+  </si>
+  <si>
+    <t>Acero - De La Cruz</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Chicago Math &amp; Science Hs</t>
+  </si>
+  <si>
+    <t>Kilmer</t>
+  </si>
+  <si>
+    <t>New Field</t>
+  </si>
+  <si>
+    <t>Hartigan (David) Beach</t>
+  </si>
+  <si>
+    <t>Howard (Ure) Beach</t>
+  </si>
+  <si>
+    <t>Griffin (Marion Mahony) Beach</t>
+  </si>
+  <si>
+    <t>Langdon (Mary Margaret)</t>
+  </si>
+  <si>
+    <t>Lazarus (Emma)</t>
+  </si>
+  <si>
+    <t>Leone (Sam) Beach</t>
+  </si>
+  <si>
+    <t>Loyola</t>
+  </si>
+  <si>
+    <t>Columbia Beach</t>
+  </si>
+  <si>
+    <t>Matanky (Eugene)</t>
+  </si>
+  <si>
+    <t>Fargo (James) Beach</t>
+  </si>
+  <si>
+    <t>Goldberg (Louis)</t>
+  </si>
+  <si>
+    <t>Paschen (Christian)</t>
+  </si>
+  <si>
+    <t>White (Willye B.)</t>
+  </si>
+  <si>
+    <t>Pottawattomie</t>
+  </si>
+  <si>
+    <t>Juneway Terr. Beach</t>
+  </si>
+  <si>
+    <t>Prinz (Tobey) Beach</t>
+  </si>
+  <si>
+    <t>North Shore Beach</t>
+  </si>
+  <si>
+    <t>Rogers (Phillip) Beach</t>
+  </si>
+  <si>
+    <t>Touhy (Patrick)</t>
+  </si>
+  <si>
+    <t>Washington (Harold) Mem.</t>
+  </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>Dubkin (Leonard)</t>
+  </si>
+  <si>
+    <t>E102</t>
   </si>
   <si>
     <t>6907 N. Clark St.</t>
   </si>
   <si>
-    <t>6631 N BOSWORTH AVE</t>
-  </si>
-  <si>
-    <t>1631 W JONQUIL TER</t>
-  </si>
-  <si>
-    <t>7416 N RIDGE BLVD</t>
-  </si>
-  <si>
-    <t>7019 N ASHLAND AVE</t>
-  </si>
-  <si>
-    <t>7414 N WOLCOTT AVE</t>
-  </si>
-  <si>
-    <t>7212 N CLARK ST</t>
-  </si>
-  <si>
-    <t>6700 N GREENVIEW AVE</t>
-  </si>
-  <si>
-    <t>1707 W MORSE AVE</t>
+    <t>6631 N Bosworth Ave</t>
+  </si>
+  <si>
+    <t>1631 W Jonquil Ter</t>
+  </si>
+  <si>
+    <t>7416 N Ridge Blvd</t>
+  </si>
+  <si>
+    <t>7019 N Ashland Ave</t>
+  </si>
+  <si>
+    <t>7414 N Wolcott Ave</t>
+  </si>
+  <si>
+    <t>7212 N Clark St</t>
+  </si>
+  <si>
+    <t>6700 N Greenview Ave</t>
+  </si>
+  <si>
+    <t>1707 W Morse Ave</t>
+  </si>
+  <si>
+    <t>7340 N Clark St</t>
   </si>
   <si>
     <t>Chicago</t>
@@ -199,70 +205,70 @@
     <t>Park</t>
   </si>
   <si>
+    <t>Fire Station</t>
+  </si>
+  <si>
     <t>High School</t>
   </si>
   <si>
     <t>Elementary School</t>
   </si>
   <si>
-    <t>PLAYGROUND</t>
-  </si>
-  <si>
-    <t>BEACH</t>
-  </si>
-  <si>
-    <t>PLAYGROUND PARK</t>
-  </si>
-  <si>
-    <t>GYMNASIUM</t>
-  </si>
-  <si>
-    <t>BASKETBALL COURT</t>
-  </si>
-  <si>
-    <t>FOOTBALL/SOCCER COMBO FLD</t>
-  </si>
-  <si>
-    <t>BASEBALL JR/SOFTBALL</t>
-  </si>
-  <si>
-    <t>BASEBALL SR</t>
-  </si>
-  <si>
-    <t>TENNIS COURT</t>
-  </si>
-  <si>
-    <t>BOAT LAUNCH NON-MOTORIZED</t>
-  </si>
-  <si>
-    <t>SHUFFLEBOARD</t>
-  </si>
-  <si>
-    <t>BOXING CENTER</t>
-  </si>
-  <si>
-    <t>VOLLEYBALL</t>
-  </si>
-  <si>
-    <t>HANDBALL/RACQUET (IN)</t>
-  </si>
-  <si>
-    <t>DOG FRIENDLY AREA</t>
-  </si>
-  <si>
-    <t>ARTIFICIAL TURF FIELD</t>
-  </si>
-  <si>
-    <t>NATURE/BIRD SANCTUARY</t>
-  </si>
-  <si>
-    <t>FITNESS CENTER</t>
-  </si>
-  <si>
-    <t>SPRAY FEATURE</t>
-  </si>
-  <si>
-    <t>COMMUNITY GARDEN</t>
+    <t>Playground</t>
+  </si>
+  <si>
+    <t>Beach</t>
+  </si>
+  <si>
+    <t>Gymnasium</t>
+  </si>
+  <si>
+    <t>Basketball Court</t>
+  </si>
+  <si>
+    <t>Football/Soccer Combo Fld</t>
+  </si>
+  <si>
+    <t>Baseball Jr/Softball</t>
+  </si>
+  <si>
+    <t>Baseball Sr</t>
+  </si>
+  <si>
+    <t>Tennis Court</t>
+  </si>
+  <si>
+    <t>Boat Launch Non-Motorized</t>
+  </si>
+  <si>
+    <t>Shuffleboard</t>
+  </si>
+  <si>
+    <t>Boxing Center</t>
+  </si>
+  <si>
+    <t>Volleyball</t>
+  </si>
+  <si>
+    <t>Handball/Racquet (In)</t>
+  </si>
+  <si>
+    <t>Dog Friendly Area</t>
+  </si>
+  <si>
+    <t>Artificial Turf Field</t>
+  </si>
+  <si>
+    <t>Nature/Bird Sanctuary</t>
+  </si>
+  <si>
+    <t>Fitness Center</t>
+  </si>
+  <si>
+    <t>Spray Feature</t>
+  </si>
+  <si>
+    <t>Community Garden</t>
   </si>
 </sst>
 </file>
@@ -633,7 +639,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -682,22 +688,22 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H2">
         <v>42.00670763656976</v>
@@ -706,13 +712,13 @@
         <v>-87.6734076726854</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -720,7 +726,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H3">
         <v>42.00268756</v>
@@ -729,10 +735,10 @@
         <v>-87.66919215</v>
       </c>
       <c r="K3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -740,7 +746,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H4">
         <v>42.02109056</v>
@@ -749,10 +755,10 @@
         <v>-87.67193897999999</v>
       </c>
       <c r="K4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -760,7 +766,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H5">
         <v>42.01647588</v>
@@ -769,10 +775,10 @@
         <v>-87.68440568</v>
       </c>
       <c r="K5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -780,7 +786,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H6">
         <v>42.00966386</v>
@@ -789,10 +795,10 @@
         <v>-87.6699854</v>
       </c>
       <c r="K6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L6" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -800,7 +806,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H7">
         <v>42.01708759</v>
@@ -809,10 +815,10 @@
         <v>-87.67776252</v>
       </c>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L7" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -820,7 +826,7 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H8">
         <v>42.01303149</v>
@@ -829,10 +835,10 @@
         <v>-87.67481841999999</v>
       </c>
       <c r="K8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L8" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -840,7 +846,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H9">
         <v>42.00364046</v>
@@ -849,10 +855,10 @@
         <v>-87.66822247</v>
       </c>
       <c r="K9" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -860,7 +866,7 @@
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H10">
         <v>42.00770257</v>
@@ -869,10 +875,10 @@
         <v>-87.67316833</v>
       </c>
       <c r="K10" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="L10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -886,10 +892,10 @@
         <v>-87.65769376</v>
       </c>
       <c r="K11" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L11" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -903,10 +909,10 @@
         <v>-87.66391455</v>
       </c>
       <c r="K12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -920,10 +926,10 @@
         <v>-87.66424859999999</v>
       </c>
       <c r="K13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L13" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -937,10 +943,10 @@
         <v>-87.66262924999999</v>
       </c>
       <c r="K14" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L14" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -954,10 +960,10 @@
         <v>-87.67487409</v>
       </c>
       <c r="K15" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -971,10 +977,10 @@
         <v>-87.66319003</v>
       </c>
       <c r="K16" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -988,10 +994,10 @@
         <v>-87.66156823999999</v>
       </c>
       <c r="K17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L17" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1005,10 +1011,10 @@
         <v>-87.66253502000001</v>
       </c>
       <c r="K18" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L18" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1022,10 +1028,10 @@
         <v>-87.66316225999999</v>
       </c>
       <c r="K19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L19" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1039,10 +1045,10 @@
         <v>-87.66170244</v>
       </c>
       <c r="K20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L20" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1056,10 +1062,10 @@
         <v>-87.65909651</v>
       </c>
       <c r="K21" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L21" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -1073,10 +1079,10 @@
         <v>-87.6584077</v>
       </c>
       <c r="K22" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L22" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1090,10 +1096,10 @@
         <v>-87.66159962</v>
       </c>
       <c r="K23" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L23" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -1107,10 +1113,10 @@
         <v>-87.66248470000001</v>
       </c>
       <c r="K24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L24" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -1124,10 +1130,10 @@
         <v>-87.66061040000001</v>
       </c>
       <c r="K25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L25" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:12">
@@ -1141,10 +1147,10 @@
         <v>-87.66208738</v>
       </c>
       <c r="K26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -1158,10 +1164,10 @@
         <v>-87.65816288000001</v>
       </c>
       <c r="K27" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L27" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -1175,10 +1181,10 @@
         <v>-87.66221625</v>
       </c>
       <c r="K28" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L28" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1192,10 +1198,10 @@
         <v>-87.65723976</v>
       </c>
       <c r="K29" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L29" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:12">
@@ -1209,10 +1215,10 @@
         <v>-87.68052475</v>
       </c>
       <c r="K30" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L30" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:12">
@@ -1226,10 +1232,10 @@
         <v>-87.66303859999999</v>
       </c>
       <c r="K31" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L31" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:12">
@@ -1243,10 +1249,10 @@
         <v>-87.66565974</v>
       </c>
       <c r="K32" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1260,10 +1266,10 @@
         <v>-87.66033019</v>
       </c>
       <c r="K33" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L33" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1277,10 +1283,10 @@
         <v>-87.66139119</v>
       </c>
       <c r="K34" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L34" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1294,10 +1300,10 @@
         <v>-87.67972193999999</v>
       </c>
       <c r="K35" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L35" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1311,10 +1317,10 @@
         <v>-87.67151174999999</v>
       </c>
       <c r="K36" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L36" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1328,10 +1334,10 @@
         <v>-87.67813995</v>
       </c>
       <c r="K37" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L37" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:12">
@@ -1345,10 +1351,10 @@
         <v>-87.67673435</v>
       </c>
       <c r="K38" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L38" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -1362,10 +1368,10 @@
         <v>-87.67867489</v>
       </c>
       <c r="K39" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L39" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1379,10 +1385,10 @@
         <v>-87.65640562</v>
       </c>
       <c r="K40" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L40" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:12">
@@ -1396,10 +1402,10 @@
         <v>-87.66522105</v>
       </c>
       <c r="K41" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L41" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -1413,10 +1419,10 @@
         <v>-87.65748605</v>
       </c>
       <c r="K42" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L42" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:12">
@@ -1430,10 +1436,10 @@
         <v>-87.65734402</v>
       </c>
       <c r="K43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L43" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:12">
@@ -1447,10 +1453,10 @@
         <v>-87.67992694</v>
       </c>
       <c r="K44" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L44" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -1464,10 +1470,10 @@
         <v>-87.67950729</v>
       </c>
       <c r="K45" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L45" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -1481,10 +1487,10 @@
         <v>-87.67757895</v>
       </c>
       <c r="K46" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L46" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -1498,10 +1504,10 @@
         <v>-87.67716962</v>
       </c>
       <c r="K47" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L47" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="48" spans="1:12">
@@ -1515,10 +1521,10 @@
         <v>-87.67810622</v>
       </c>
       <c r="K48" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L48" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -1532,10 +1538,10 @@
         <v>-87.67820733000001</v>
       </c>
       <c r="K49" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L49" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -1549,10 +1555,10 @@
         <v>-87.67648475</v>
       </c>
       <c r="K50" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L50" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:12">
@@ -1566,10 +1572,10 @@
         <v>-87.67859150000001</v>
       </c>
       <c r="K51" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L51" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="52" spans="1:12">
@@ -1583,10 +1589,10 @@
         <v>-87.67857954999999</v>
       </c>
       <c r="K52" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L52" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:12">
@@ -1600,10 +1606,10 @@
         <v>-87.67788145999999</v>
       </c>
       <c r="K53" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L53" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:12">
@@ -1617,10 +1623,10 @@
         <v>-87.66471496</v>
       </c>
       <c r="K54" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L54" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="1:12">
@@ -1634,10 +1640,10 @@
         <v>-87.66456614000001</v>
       </c>
       <c r="K55" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L55" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -1651,10 +1657,10 @@
         <v>-87.67360098</v>
       </c>
       <c r="K56" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L56" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="57" spans="1:12">
@@ -1668,10 +1674,10 @@
         <v>-87.67386432000001</v>
       </c>
       <c r="K57" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L57" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:12">
@@ -1685,10 +1691,10 @@
         <v>-87.67275167</v>
       </c>
       <c r="K58" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L58" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:12">
@@ -1702,10 +1708,10 @@
         <v>-87.67465871</v>
       </c>
       <c r="K59" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L59" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="60" spans="1:12">
@@ -1719,10 +1725,10 @@
         <v>-87.67338743000001</v>
       </c>
       <c r="K60" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L60" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:12">
@@ -1736,10 +1742,10 @@
         <v>-87.67154392</v>
       </c>
       <c r="K61" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L61" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:12">
@@ -1753,10 +1759,10 @@
         <v>-87.67032349999999</v>
       </c>
       <c r="K62" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L62" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="63" spans="1:12">
@@ -1770,10 +1776,10 @@
         <v>-87.67091352</v>
       </c>
       <c r="K63" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L63" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:12">
@@ -1787,10 +1793,10 @@
         <v>-87.67136621</v>
       </c>
       <c r="K64" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L64" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="65" spans="1:12">
@@ -1804,10 +1810,10 @@
         <v>-87.67446021000001</v>
       </c>
       <c r="K65" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L65" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:12">
@@ -1821,10 +1827,10 @@
         <v>-87.67065533</v>
       </c>
       <c r="K66" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L66" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:12">
@@ -1838,10 +1844,10 @@
         <v>-87.665638</v>
       </c>
       <c r="K67" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L67" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="68" spans="1:12">
@@ -1855,10 +1861,39 @@
         <v>-87.65960633</v>
       </c>
       <c r="K68" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L68" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12">
+      <c r="A69" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69" t="s">
+        <v>54</v>
+      </c>
+      <c r="D69" t="s">
+        <v>55</v>
+      </c>
+      <c r="E69" t="s">
+        <v>56</v>
+      </c>
+      <c r="H69">
+        <v>42.01464016068629</v>
+      </c>
+      <c r="I69">
+        <v>-87.67502361090746</v>
+      </c>
+      <c r="K69" t="s">
+        <v>63</v>
+      </c>
+      <c r="L69" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>